<commit_message>
fix bug in radtags shell
</commit_message>
<xml_diff>
--- a/scripts/barcodes_KGoriginal_file.xlsx
+++ b/scripts/barcodes_KGoriginal_file.xlsx
@@ -4246,10 +4246,10 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="B1:P48"/>
+  <dimension ref="B1:R48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+      <selection activeCell="R27" sqref="R27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4688,7 +4688,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>305</v>
       </c>
@@ -4714,7 +4714,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>306</v>
       </c>
@@ -4740,7 +4740,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>307</v>
       </c>
@@ -4766,7 +4766,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>308</v>
       </c>
@@ -4792,7 +4792,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>309</v>
       </c>
@@ -4818,7 +4818,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>310</v>
       </c>
@@ -4844,7 +4844,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>311</v>
       </c>
@@ -4870,7 +4870,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>312</v>
       </c>
@@ -4896,7 +4896,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>313</v>
       </c>
@@ -4922,7 +4922,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>314</v>
       </c>
@@ -4947,8 +4947,12 @@
       <c r="P26" t="s">
         <v>760</v>
       </c>
-    </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="R26">
+        <f>425-377</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>315</v>
       </c>
@@ -4974,7 +4978,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>316</v>
       </c>
@@ -5000,7 +5004,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>317</v>
       </c>
@@ -5026,7 +5030,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>318</v>
       </c>
@@ -5052,7 +5056,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>319</v>
       </c>
@@ -5078,7 +5082,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>320</v>
       </c>

</xml_diff>